<commit_message>
se agregaron y actualizaron la matriz de rastreo y plan de prueba
</commit_message>
<xml_diff>
--- a/DMS_A4_MATRIZ_DE_RASTREO/DMS_A4_PT1_MATRIZ_DE_RASTREO.xlsx
+++ b/DMS_A4_MATRIZ_DE_RASTREO/DMS_A4_PT1_MATRIZ_DE_RASTREO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="48">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Diagrama de clases</t>
   </si>
   <si>
-    <t>Diagrama de secuencia</t>
-  </si>
-  <si>
     <t>Modelo lógico</t>
   </si>
   <si>
@@ -136,21 +133,6 @@
     <t>Córdoba,Ver.</t>
   </si>
   <si>
-    <t>Módulo Clientes</t>
-  </si>
-  <si>
-    <t>Módulo Cotizaciones</t>
-  </si>
-  <si>
-    <t>Módulo Herramientas</t>
-  </si>
-  <si>
-    <t>Módulo Ingresos y Egresos</t>
-  </si>
-  <si>
-    <t>Módulo Personal</t>
-  </si>
-  <si>
     <t>Módulo productos</t>
   </si>
   <si>
@@ -164,6 +146,24 @@
   </si>
   <si>
     <t>Modelo</t>
+  </si>
+  <si>
+    <t>Módulo personal</t>
+  </si>
+  <si>
+    <t>Módulo ingresos y egresos</t>
+  </si>
+  <si>
+    <t>Módulo herramientas</t>
+  </si>
+  <si>
+    <t>Módulo cotizaciones</t>
+  </si>
+  <si>
+    <t>Módulo clientes</t>
+  </si>
+  <si>
+    <t>Módulo inicio de sesión</t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -332,11 +332,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -396,6 +409,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -438,17 +460,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -928,114 +956,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="25" t="s">
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="25" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="29">
+      <c r="D3" s="30"/>
+      <c r="E3" s="34">
         <v>41869</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1062,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB39"/>
+  <dimension ref="A1:AC40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E20"/>
+    <sheetView tabSelected="1" topLeftCell="S5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1073,37 +1101,37 @@
     <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="26" width="15.42578125" customWidth="1"/>
+    <col min="5" max="27" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -1117,14 +1145,14 @@
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
+      <c r="B5" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -1139,30 +1167,30 @@
       <c r="D6" s="12">
         <v>41869</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="35"/>
+      <c r="F6" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:28" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
+        <v>36</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
@@ -1189,77 +1217,79 @@
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="40" t="s">
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="40"/>
-      <c r="S10" s="40"/>
-      <c r="T10" s="40"/>
-      <c r="U10" s="40"/>
-      <c r="V10" s="40"/>
-      <c r="W10" s="40"/>
-      <c r="X10" s="40" t="s">
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="47"/>
+      <c r="W10" s="47"/>
+      <c r="X10" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="Y10" s="40"/>
-      <c r="Z10" s="40"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="48"/>
+      <c r="AA10" s="29"/>
     </row>
     <row r="11" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
-      <c r="B11" s="39" t="s">
+      <c r="A11" s="42"/>
+      <c r="B11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40" t="s">
+      <c r="C11" s="45"/>
+      <c r="D11" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40" t="s">
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="42"/>
-      <c r="V11" s="42"/>
-      <c r="W11" s="42"/>
-      <c r="X11" s="8"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="47"/>
+      <c r="W11" s="47"/>
+      <c r="X11" s="27"/>
       <c r="Y11" s="8"/>
       <c r="Z11" s="8"/>
+      <c r="AA11" s="29"/>
     </row>
     <row r="12" spans="1:28" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="20" t="s">
         <v>18</v>
       </c>
@@ -1270,13 +1300,13 @@
         <v>20</v>
       </c>
       <c r="E12" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>21</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>46</v>
       </c>
       <c r="H12" s="20" t="s">
         <v>22</v>
@@ -1290,9 +1320,7 @@
       <c r="K12" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="L12" s="20"/>
       <c r="M12" s="20"/>
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
@@ -1305,52 +1333,51 @@
       <c r="V12" s="20"/>
       <c r="W12" s="20"/>
       <c r="X12" s="20" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="Y12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z12" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Z12" s="20" t="s">
-        <v>31</v>
-      </c>
+      <c r="AA12" s="29"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="21" t="s">
         <v>28</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="21" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L13" s="21"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
       <c r="O13" s="21"/>
@@ -1363,54 +1390,52 @@
       <c r="V13" s="21"/>
       <c r="W13" s="21"/>
       <c r="X13" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y13" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z13" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA13" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="AA13" s="29"/>
       <c r="AB13" s="10"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="21" t="s">
         <v>28</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" s="21" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
       <c r="O14" s="21"/>
@@ -1423,54 +1448,52 @@
       <c r="V14" s="21"/>
       <c r="W14" s="21"/>
       <c r="X14" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y14" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z14" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA14" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="AA14" s="29"/>
       <c r="AB14" s="10"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="21" t="s">
         <v>28</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
       <c r="O15" s="21"/>
@@ -1483,54 +1506,52 @@
       <c r="V15" s="21"/>
       <c r="W15" s="21"/>
       <c r="X15" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y15" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z15" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA15" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="AA15" s="29"/>
       <c r="AB15" s="10"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="21" t="s">
         <v>28</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K16" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
       <c r="O16" s="21"/>
@@ -1543,54 +1564,52 @@
       <c r="V16" s="21"/>
       <c r="W16" s="21"/>
       <c r="X16" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y16" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z16" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA16" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="AA16" s="29"/>
       <c r="AB16" s="10"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="21" t="s">
         <v>28</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K17" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" s="21" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
       <c r="O17" s="21"/>
@@ -1603,54 +1622,52 @@
       <c r="V17" s="21"/>
       <c r="W17" s="21"/>
       <c r="X17" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y17" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z17" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA17" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="AA17" s="29"/>
       <c r="AB17" s="10"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="21" t="s">
         <v>28</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J18" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K18" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="21" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
       <c r="O18" s="21"/>
@@ -1663,54 +1680,52 @@
       <c r="V18" s="21"/>
       <c r="W18" s="21"/>
       <c r="X18" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Y18" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z18" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA18" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="AA18" s="28"/>
       <c r="AB18" s="10"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>28</v>
+        <v>47</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="21" t="s">
         <v>28</v>
       </c>
       <c r="H19" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K19" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="21" t="s">
-        <v>28</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L19" s="21"/>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
       <c r="O19" s="21"/>
@@ -1723,136 +1738,165 @@
       <c r="V19" s="21"/>
       <c r="W19" s="21"/>
       <c r="X19" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y19" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z19" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA19" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="AA19" s="19"/>
       <c r="AB19" s="10"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
+        <v>27</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="21"/>
       <c r="X20" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y20" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Z20" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA20" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="AA20" s="19"/>
       <c r="AB20" s="10"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="16"/>
-      <c r="Z21" s="16"/>
-      <c r="AA21" s="10"/>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA21" s="19"/>
       <c r="AB21" s="10"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="19"/>
-      <c r="V22" s="19"/>
-      <c r="W22" s="19"/>
-      <c r="X22" s="19"/>
-      <c r="Y22" s="19"/>
-      <c r="Z22" s="19"/>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="16"/>
+      <c r="Z22" s="16"/>
+      <c r="AA22" s="19"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -1879,8 +1923,9 @@
       <c r="X23" s="19"/>
       <c r="Y23" s="19"/>
       <c r="Z23" s="19"/>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA23" s="19"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -1907,8 +1952,9 @@
       <c r="X24" s="19"/>
       <c r="Y24" s="19"/>
       <c r="Z24" s="19"/>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA24" s="19"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -1935,8 +1981,9 @@
       <c r="X25" s="19"/>
       <c r="Y25" s="19"/>
       <c r="Z25" s="19"/>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA25" s="19"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -1963,8 +2010,9 @@
       <c r="X26" s="19"/>
       <c r="Y26" s="19"/>
       <c r="Z26" s="19"/>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA26" s="19"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -1991,8 +2039,9 @@
       <c r="X27" s="19"/>
       <c r="Y27" s="19"/>
       <c r="Z27" s="19"/>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA27" s="19"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -2019,8 +2068,9 @@
       <c r="X28" s="19"/>
       <c r="Y28" s="19"/>
       <c r="Z28" s="19"/>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA28" s="19"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
@@ -2047,8 +2097,9 @@
       <c r="X29" s="19"/>
       <c r="Y29" s="19"/>
       <c r="Z29" s="19"/>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA29" s="19"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
@@ -2075,8 +2126,9 @@
       <c r="X30" s="19"/>
       <c r="Y30" s="19"/>
       <c r="Z30" s="19"/>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA30" s="19"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -2103,8 +2155,9 @@
       <c r="X31" s="19"/>
       <c r="Y31" s="19"/>
       <c r="Z31" s="19"/>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA31" s="19"/>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -2131,8 +2184,9 @@
       <c r="X32" s="19"/>
       <c r="Y32" s="19"/>
       <c r="Z32" s="19"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA32" s="19"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -2159,8 +2213,9 @@
       <c r="X33" s="19"/>
       <c r="Y33" s="19"/>
       <c r="Z33" s="19"/>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA33" s="19"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -2187,8 +2242,9 @@
       <c r="X34" s="19"/>
       <c r="Y34" s="19"/>
       <c r="Z34" s="19"/>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA34" s="19"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -2216,7 +2272,7 @@
       <c r="Y35" s="19"/>
       <c r="Z35" s="19"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -2244,7 +2300,7 @@
       <c r="Y36" s="19"/>
       <c r="Z36" s="19"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -2272,23 +2328,51 @@
       <c r="Y37" s="19"/>
       <c r="Z37" s="19"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A38" s="17"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+      <c r="Y38" s="19"/>
+      <c r="Z38" s="19"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A40" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="M10:W10"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="L11:W11"/>
+    <mergeCell ref="L10:W10"/>
     <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="M11:W11"/>
     <mergeCell ref="A1:G3"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:G7"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:K11"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>